<commit_message>
new examples and output
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,34 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25524"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="429" documentId="11_98E204A94376DF869BFAB765370305E98403B110" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0DB87B0-167E-4F23-92EA-14B9FD08DA2F}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\diagrams.R\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E11CF3D-67CB-4848-97EE-83CE1E252C7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="107">
   <si>
     <t>status</t>
   </si>
@@ -108,7 +101,13 @@
     <t>01_T2_1_022_CreateItemSetDatasets</t>
   </si>
   <si>
-    <t>SURVEY_OBSERVATIONS, MEDICAL_OBSERVATIONS</t>
+    <t>promptsetdataset</t>
+  </si>
+  <si>
+    <t>01_T2_1_022_CreatePromptSetDatasets</t>
+  </si>
+  <si>
+    <t>SURVEY_ID VISIT_OCCURRENCE_ID</t>
   </si>
   <si>
     <t>D3_clean_spells</t>
@@ -129,10 +128,22 @@
     <t>D3_vaccines_curated</t>
   </si>
   <si>
+    <t>01_T2_05_apply_criteria_for_doses.R</t>
+  </si>
+  <si>
     <t>D3_selection_criteria_from_PERSON_to_study_population</t>
   </si>
   <si>
-    <t>01_T2_05_selection_criteria_from_PERSON_to_study_population.R</t>
+    <t>01_T2_06_selection_criteria_from_PERSON_to_study_population.R</t>
+  </si>
+  <si>
+    <t>PERSONS D3_vaccines_curated D3_output_spells_category D3_persons</t>
+  </si>
+  <si>
+    <t>D3_selection_criteria_from_PERSONS_to_children_study_population</t>
+  </si>
+  <si>
+    <t>01_T2_06_selection_criteria_from_PERSON_to_children_study_population.R</t>
   </si>
   <si>
     <t>D4_study_population</t>
@@ -141,15 +152,12 @@
     <t>02_T3_01_create_study_population.R</t>
   </si>
   <si>
+    <t>D4_children_study_population</t>
+  </si>
+  <si>
     <t>D3_selection_criteria_from_PERSONS_to_unmatched_children_study_population</t>
   </si>
   <si>
-    <t>01_T2_06_selection_criteria_from_PERSON_to_unmatched_children_study_population.R</t>
-  </si>
-  <si>
-    <t>D4_unmatched_children_study_population</t>
-  </si>
-  <si>
     <t>UMCU coding</t>
   </si>
   <si>
@@ -159,6 +167,9 @@
     <t>03_T2_01_create_D3_covid_episodes</t>
   </si>
   <si>
+    <t>itemsetdataset conceptsetdataset promptsetdataset</t>
+  </si>
+  <si>
     <t>D3_covid_sev2</t>
   </si>
   <si>
@@ -171,55 +182,114 @@
     <t>03_T2_03_create_D3_covid_sev3</t>
   </si>
   <si>
+    <t>itemsetdataset conceptsetdataset promptsetdataset D3_persons</t>
+  </si>
+  <si>
     <t>D3_outcomes</t>
   </si>
   <si>
     <t>03_T2_04_create_D3_outcomes</t>
   </si>
   <si>
+    <t>D3_covid_episodes D3_covid_sev2 D3_covid_sev3 D3_death</t>
+  </si>
+  <si>
+    <t>D3_contacts_with_health_system_past_7_days_TD</t>
+  </si>
+  <si>
+    <t>04_T2_01_create_time_dependent_matching_variable.R</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">D4_study_population </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>promptsetdataset</t>
+    </r>
+  </si>
+  <si>
+    <t>D3_last_covid_TD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">D4_study_population </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>conceptsetdataset</t>
+    </r>
+  </si>
+  <si>
+    <t>D3_ageband_TD</t>
+  </si>
+  <si>
+    <t>D3_immunodeficiency_TD</t>
+  </si>
+  <si>
+    <t>D3_cancer_TD</t>
+  </si>
+  <si>
+    <t>D3_Im_TRANSPLANTRECIPIENT_COV_TD</t>
+  </si>
+  <si>
+    <t>D3_G_SEVERERENALDISEASE_CH_TD</t>
+  </si>
+  <si>
+    <t>D3_O_DOWN_COV_TD</t>
+  </si>
+  <si>
     <t>D3_study_population_with_matching_variables</t>
   </si>
   <si>
-    <t>04_T2_01_create_study_population_with_matching_variables.R</t>
+    <t>04_T2_02_create_study_population_with_matching_variables.R</t>
   </si>
   <si>
     <t>D3_persons D4_study_population D3_vaccines_curated D3_covid_episodes</t>
   </si>
   <si>
-    <t>end_of_stud</t>
-  </si>
-  <si>
-    <t>D3_unmatched_children_study_population_with_matching_variables</t>
-  </si>
-  <si>
-    <t>04_T2_02_create_unmatched_children_study_population_with_matching_variables.R</t>
-  </si>
-  <si>
-    <t>D4_unmatched_children_study_population D3_vaccines_curated D3_covid_episodes</t>
-  </si>
-  <si>
-    <t>D3_no_contacts_with_health_system_past_7_days</t>
-  </si>
-  <si>
-    <t>04_T2_03_create_time_dependent_matching_variable.R</t>
-  </si>
-  <si>
-    <t>D3_covid_episodes_past_6months</t>
-  </si>
-  <si>
-    <t>D4_matched_HO_P_to_HE_P_study_population</t>
+    <t>D3_children_study_population_with_matching_variables</t>
+  </si>
+  <si>
+    <t>04_T2_03_create_children_study_population_with_matching_variables.R</t>
+  </si>
+  <si>
+    <t>D4_children_study_population D3_vaccines_curated D3_covid_episodes</t>
+  </si>
+  <si>
+    <t>D4_HO_P_to_HE_P_pairs_and_unmatched</t>
   </si>
   <si>
     <t>05_T3_01_match_HO_P_to_HE_P.R</t>
   </si>
   <si>
-    <t>D3_study_population_with_matching_variables D3_covid_episodes_past_6months D3_no_contacts_with_health_system_past_7_days</t>
+    <t>D3_study_population_with_matching_variables D3_last_covid_TD D3_ageband_TD D3_immunodeficiency_TD D3_cancer_TD D3_Im_TRANSPLANTRECIPIENT_COV_TD D3_G_SEVERERENALDISEASE_CH_TD D3_O_DOWN_COV_TD</t>
   </si>
   <si>
     <t>protocol section 8.4.2</t>
   </si>
   <si>
-    <t>D4_matched_HO_P_HO_B_to_NB_study_population</t>
+    <t>D4_HO_P_HO_B_to_NB_pairs_and_unmatched</t>
   </si>
   <si>
     <t>05_T3_02_match_HO_P_HO_B_to_NB.R</t>
@@ -228,7 +298,7 @@
     <t>8.4.3 sub 1.1</t>
   </si>
   <si>
-    <t>D4_matched_HO_P_HE_B_to_NB_study_population</t>
+    <t>D4_HO_P_HE_B_to_NB_pairs_and_unmatched</t>
   </si>
   <si>
     <t>05_T3_03_match_HO_P_HE_B_to_NB.R</t>
@@ -237,7 +307,7 @@
     <t>8.4.3 sub 1.2</t>
   </si>
   <si>
-    <t>D4_matched_HE_P_B_to_NB_study_population</t>
+    <t>D4_HE_P_B_to_NB_pairs_and_unmatched</t>
   </si>
   <si>
     <t>05_T3_04_match_HE_P_B_to_NB.R</t>
@@ -246,16 +316,19 @@
     <t>8.4.3 sub 1.3</t>
   </si>
   <si>
-    <t>D4_matched_ANY_P_with_prior_covid_B_to_NB_study_population</t>
+    <t>D4_ANY_P_with_prior_covid_B_to_NB_pairs_and_unmatched</t>
   </si>
   <si>
     <t>05_T3_05_match_ANY_P_with_prior_covid_B_to_NB.R</t>
   </si>
   <si>
+    <t>D3_children_population_with_matching_variables D3_last_covid_TD D3_ageband_TD D3_immunodeficiency_TD D3_cancer_TD D3_Im_TRANSPLANTRECIPIENT_COV_TD D3_G_SEVERERENALDISEASE_CH_TD D3_O_DOWN_COV_TD</t>
+  </si>
+  <si>
     <t>8.4.3 sub 1.4</t>
   </si>
   <si>
-    <t>D4_matched_children_study_population</t>
+    <t>D4_children_study_pairs_and_unmatched</t>
   </si>
   <si>
     <t>05_T3_06_match_children.R</t>
@@ -267,6 +340,25 @@
     <t>06_T2_01_create_main_variables_for_matched_study_population.R</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">D4_HO_P_to_HE_P_pairs_and_unmatched D4_HO_P_HO_B_to_NB_pairs_and_unmatched D4_HO_P_HE_B_to_NB_pairs_and_unmatched D4_HE_P_B_to_NB_pairs_and_unmatched D4_ANY_P_with_prior_covid_B_to_NB_pairs_and_unmatched D4_children_study_pairs_and_unmatched </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>conceptsetdataset</t>
+    </r>
+  </si>
+  <si>
     <t>D4_HO_P_to_HE_P_analytic_dataset</t>
   </si>
   <si>
@@ -295,13 +387,16 @@
   </si>
   <si>
     <t>values</t>
+  </si>
+  <si>
+    <t>SURVEY_OBSERVATIONS MEDICAL_OBSERVATIONS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,8 +438,27 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -354,6 +468,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,12 +490,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -388,6 +505,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,17 +831,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="F2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="5" max="5" width="52.42578125" customWidth="1"/>
     <col min="6" max="6" width="89.42578125" customWidth="1"/>
     <col min="7" max="7" width="38.5703125" customWidth="1"/>
     <col min="8" max="8" width="36.5703125" customWidth="1"/>
@@ -720,39 +851,39 @@
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -772,7 +903,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -792,7 +923,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -802,7 +933,7 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
@@ -812,7 +943,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -822,19 +953,19 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -842,18 +973,17 @@
       <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>28</v>
       </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -863,32 +993,38 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
+      <c r="D7" s="1"/>
       <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
         <v>30</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>33</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -898,14 +1034,17 @@
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>33</v>
+      <c r="E9" t="s">
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -915,459 +1054,638 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" t="s">
-        <v>35</v>
+      <c r="E10" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="6" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="H13" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>47</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>50</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>47</v>
+      <c r="E16" t="s">
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
       </c>
       <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="6" t="s">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7" t="s">
+      <c r="F18" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
+      <c r="H18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="6" t="s">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H21" t="s">
+      <c r="F19" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="J21" t="s">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
+      <c r="F20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H22" t="s">
+      <c r="F22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="J22" t="s">
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="16" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F24" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H23" t="s">
+      <c r="F25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="J23" t="s">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
+      <c r="F26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="H26" t="s">
         <v>70</v>
       </c>
-      <c r="H24" t="s">
-        <v>61</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
+      <c r="F27" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="H27" t="s">
         <v>73</v>
       </c>
-      <c r="H25" t="s">
-        <v>61</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6" t="s">
+      <c r="F28" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="H28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
+      <c r="J28" t="s">
         <v>77</v>
       </c>
-      <c r="F28" s="9" t="s">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
+      <c r="F29" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="H29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
+      <c r="F30" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
+      <c r="H30" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6" t="s">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="H31" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H32" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1383,26 +1701,26 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1669,13 +1987,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cdb8be3a-47f3-4316-ba45-a9ae8c99e520"/>
+    <ds:schemaRef ds:uri="6ebf3131-fd27-47ae-a3c2-4b1866324e6f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71CB1746-6380-42C1-8645-2A7AC9196E41}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71CB1746-6380-42C1-8645-2A7AC9196E41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ebf3131-fd27-47ae-a3c2-4b1866324e6f"/>
+    <ds:schemaRef ds:uri="cdb8be3a-47f3-4316-ba45-a9ae8c99e520"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>